<commit_message>
Added a time record
</commit_message>
<xml_diff>
--- a/game time.xlsx
+++ b/game time.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Program Files\HTML\Games\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{003D61DB-5B17-464D-B789-38002786D79C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E01EA80F-822B-46BF-89B0-A11DBB7E193B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2535" yWindow="1590" windowWidth="21600" windowHeight="12555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>Игра</t>
   </si>
@@ -163,6 +163,15 @@
   </si>
   <si>
     <t>Life is Strange</t>
+  </si>
+  <si>
+    <t>Grand Theft Auto Online</t>
+  </si>
+  <si>
+    <t>Life is Strange: Before The Storm</t>
+  </si>
+  <si>
+    <t>Beyond: Two Souls</t>
   </si>
 </sst>
 </file>
@@ -573,10 +582,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="J39" sqref="J39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,359 +613,356 @@
     </row>
     <row r="2" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="7">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="C2" s="8">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="D2" s="9">
-        <v>58.9</v>
+        <v>89.733333333333306</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B3" s="7">
-        <v>21</v>
+        <v>75</v>
       </c>
       <c r="C3" s="8">
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="D3" s="9">
-        <v>48.966666666666598</v>
+        <v>58.9</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="B4" s="7">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="C4" s="8">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D4" s="9">
-        <v>39.516666666666602</v>
+        <v>48.966666666666598</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>42</v>
+        <v>3</v>
+      </c>
+      <c r="B5" s="7">
+        <v>48</v>
       </c>
       <c r="C5" s="8">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="D5" s="9">
-        <v>35.41666</v>
+        <v>39.516666666666602</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="7">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="C6" s="8">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="D6" s="9">
-        <v>23.933333333333302</v>
+        <v>35.41666</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B7" s="7">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C7" s="8">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D7" s="9">
-        <v>22.5833333333333</v>
+        <v>23.933333333333302</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B8" s="7">
         <v>21</v>
       </c>
       <c r="C8" s="8">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D8" s="9">
-        <v>21.85</v>
+        <v>22.5833333333333</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="B9" s="7">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C9" s="8">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D9" s="9">
-        <v>21.65</v>
+        <v>21.85</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="B10" s="7">
         <v>19</v>
       </c>
       <c r="C10" s="8">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D10" s="9">
-        <v>21.216666666666601</v>
+        <v>21.65</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="B11" s="7">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C11" s="8">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D11" s="9">
-        <v>20.8333333333333</v>
+        <v>21.216666666666601</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B12" s="7">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="C12" s="8">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="D12" s="9">
-        <v>20.3333333333333</v>
+        <v>20.8333333333333</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B13" s="7">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="C13" s="8">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="D13" s="9">
-        <v>19.9166666666666</v>
+        <v>20.3333333333333</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="B14" s="7">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C14" s="8">
         <v>26</v>
       </c>
       <c r="D14" s="9">
-        <v>19.533333333333299</v>
+        <v>19.9166666666666</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="B15" s="7">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="C15" s="8">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="D15" s="9">
-        <v>18.183333333333302</v>
+        <v>19.533333333333299</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B16" s="7">
+        <v>8</v>
+      </c>
+      <c r="C16" s="8">
         <v>10</v>
       </c>
-      <c r="C16" s="8">
-        <v>21</v>
-      </c>
       <c r="D16" s="9">
-        <v>17.5833333333333</v>
+        <v>18.183333333333302</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="B17" s="7">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C17" s="8">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D17" s="9">
-        <v>15.25</v>
+        <v>17.5833333333333</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>44</v>
+        <v>38</v>
+      </c>
+      <c r="B18" s="7">
+        <v>16</v>
       </c>
       <c r="C18" s="8">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D18" s="9">
-        <v>15.05</v>
+        <v>15.25</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" s="7">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="C19" s="8">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D19" s="9">
-        <v>14.6</v>
+        <v>15.05</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="B20" s="7">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C20" s="8">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D20" s="9">
-        <v>13.4166666666666</v>
+        <v>14.6</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="B21" s="7">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C21" s="8">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D21" s="9">
-        <v>13.233333333333301</v>
+        <v>13.4166666666666</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B22" s="7">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C22" s="8">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D22" s="9">
-        <v>13.1166666666666</v>
+        <v>13.233333333333301</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>43</v>
+        <v>30</v>
+      </c>
+      <c r="B23" s="7">
+        <v>14</v>
       </c>
       <c r="C23" s="8">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D23" s="9">
-        <v>12.5833333333333</v>
+        <v>13.1166666666666</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B24" s="7">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="C24" s="8">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D24" s="9">
-        <v>12.283333333333299</v>
+        <v>12.5833333333333</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>45</v>
+        <v>5</v>
+      </c>
+      <c r="B25" s="7">
+        <v>8</v>
       </c>
       <c r="C25" s="8">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D25" s="9">
-        <v>11.8333333333333</v>
+        <v>12.283333333333299</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B26" s="7">
-        <v>13</v>
+        <v>45</v>
       </c>
       <c r="C26" s="8">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D26" s="9">
-        <v>10.966666666666599</v>
+        <v>11.8333333333333</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B27" s="7">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C27" s="8">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D27" s="9">
-        <v>9.85</v>
+        <v>10.966666666666599</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="B28" s="7">
         <v>11</v>
@@ -965,54 +971,51 @@
         <v>11</v>
       </c>
       <c r="D28" s="9">
-        <v>9.4166666666666607</v>
+        <v>9.85</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B29" s="7">
         <v>11</v>
       </c>
       <c r="C29" s="8">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D29" s="9">
-        <v>9.3333333333333304</v>
+        <v>9.4166666666666607</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="B30" s="7">
         <v>11</v>
       </c>
       <c r="C30" s="8">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D30" s="9">
-        <v>8.7333333333333307</v>
+        <v>9.3333333333333304</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B31" s="7">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="C31" s="8">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D31" s="9">
-        <v>8.43333333333333</v>
+        <v>8.75</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="B32" s="7">
         <v>11</v>
@@ -1021,160 +1024,199 @@
         <v>11</v>
       </c>
       <c r="D32" s="9">
-        <v>7.95</v>
+        <v>8.7333333333333307</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B33" s="7">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C33" s="8">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D33" s="9">
-        <v>7.7166666666666597</v>
+        <v>8.43333333333333</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C34" s="8">
         <v>10</v>
       </c>
       <c r="D34" s="9">
-        <v>7.4166666666666599</v>
+        <v>8.0500000000000007</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="B35" s="7">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C35" s="8">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D35" s="9">
-        <v>7.2166666666666597</v>
+        <v>7.95</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>40</v>
+        <v>22</v>
+      </c>
+      <c r="B36" s="7">
+        <v>9</v>
       </c>
       <c r="C36" s="8">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D36" s="9">
-        <v>5.55</v>
+        <v>7.7166666666666597</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B37" s="7">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="C37" s="8">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D37" s="9">
-        <v>5.3833333333333302</v>
+        <v>7.4166666666666599</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="B38" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C38" s="8">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D38" s="9">
-        <v>5.36666666666666</v>
+        <v>7.2166666666666597</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B39" s="7">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="C39" s="8">
         <v>7</v>
       </c>
       <c r="D39" s="9">
-        <v>5.0166666666666604</v>
+        <v>5.55</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="B40" s="7">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C40" s="8">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D40" s="9">
-        <v>4.93333333333333</v>
+        <v>5.3833333333333302</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="B41" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C41" s="8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D41" s="9">
-        <v>3.85</v>
+        <v>5.36666666666666</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="B42" s="7">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C42" s="8">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D42" s="9">
-        <v>3.1</v>
+        <v>5.0166666666666604</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B43" s="7">
+        <v>5</v>
+      </c>
+      <c r="C43" s="8">
+        <v>5</v>
+      </c>
+      <c r="D43" s="9">
+        <v>4.93333333333333</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B44" s="7">
+        <v>5</v>
+      </c>
+      <c r="C44" s="8">
+        <v>5</v>
+      </c>
+      <c r="D44" s="9">
+        <v>3.85</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B45" s="7">
+        <v>2</v>
+      </c>
+      <c r="C45" s="8">
+        <v>3</v>
+      </c>
+      <c r="D45" s="9">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B43" s="7">
+      <c r="B46" s="7">
         <v>4</v>
       </c>
-      <c r="C43" s="8">
+      <c r="C46" s="8">
         <v>4</v>
       </c>
-      <c r="D43" s="9">
+      <c r="D46" s="9">
         <v>2.65</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D43">
-    <sortCondition descending="1" ref="D19:D43"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D46">
+    <sortCondition descending="1" ref="D25:D46"/>
   </sortState>
   <conditionalFormatting sqref="D1:D1048576">
     <cfRule type="colorScale" priority="2">

</xml_diff>

<commit_message>
add automacy mkdir modal char input time converting
</commit_message>
<xml_diff>
--- a/game time.xlsx
+++ b/game time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Program Files\HTML\Games\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AA52C6F-7DFB-485B-A6E4-224F82967874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7260B3AD-3F00-4D2B-98C0-7E62890C425B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>Игра</t>
   </si>
@@ -196,6 +196,27 @@
   </si>
   <si>
     <t>Resident Evil 7</t>
+  </si>
+  <si>
+    <t>Cuphead</t>
+  </si>
+  <si>
+    <t>Minecraft: Восхождение</t>
+  </si>
+  <si>
+    <t>S.T.A.L.K.E.R.: Lost Alpha DC Extended</t>
+  </si>
+  <si>
+    <t>S.T.A.L.K.E.R. Lost Alpha Enhanced Edition</t>
+  </si>
+  <si>
+    <t>Cyberpunk 2077</t>
+  </si>
+  <si>
+    <t>Death Stranding</t>
+  </si>
+  <si>
+    <t>Outer Wilds</t>
   </si>
 </sst>
 </file>
@@ -606,10 +627,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D54"/>
+  <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="G66" sqref="G66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -637,497 +658,491 @@
     </row>
     <row r="2" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="C2" s="8">
-        <v>78</v>
+        <v>25</v>
       </c>
       <c r="D2" s="9">
-        <v>89.733333333333306</v>
+        <v>94.633333333333297</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="7">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="C3" s="8">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="D3" s="9">
-        <v>58.9</v>
+        <v>89.733333333333306</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B4" s="7">
-        <v>21</v>
+        <v>75</v>
       </c>
       <c r="C4" s="8">
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="D4" s="9">
-        <v>48.966666666666598</v>
+        <v>58.9</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>51</v>
+        <v>35</v>
+      </c>
+      <c r="B5" s="7">
+        <v>21</v>
       </c>
       <c r="C5" s="8">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="D5" s="9">
-        <v>45.15</v>
+        <v>48.966666666666598</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C6" s="8">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D6" s="9">
-        <v>41.116666666666603</v>
+        <v>45.15</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="7">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="C7" s="8">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="D7" s="9">
-        <v>39.516666666666602</v>
+        <v>41.116666666666603</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>42</v>
+        <v>3</v>
+      </c>
+      <c r="B8" s="7">
+        <v>48</v>
       </c>
       <c r="C8" s="8">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="D8" s="9">
-        <v>35.41666</v>
+        <v>39.516666666666602</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="C9" s="8">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="D9" s="9">
-        <v>33.6666666666666</v>
+        <v>39.35</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="7">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="C10" s="8">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="D10" s="9">
-        <v>23.933333333333302</v>
+        <v>35.41666</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="7">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="C11" s="8">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D11" s="9">
-        <v>22.5833333333333</v>
+        <v>33.6666666666666</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B12" s="7">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C12" s="8">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D12" s="9">
-        <v>21.85</v>
+        <v>23.933333333333302</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="B13" s="7">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C13" s="8">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D13" s="9">
-        <v>21.65</v>
+        <v>22.5833333333333</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>54</v>
+        <v>16</v>
+      </c>
+      <c r="B14" s="7">
+        <v>21</v>
       </c>
       <c r="C14" s="8">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D14" s="9">
-        <v>21.516666666666602</v>
+        <v>21.85</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="B15" s="7">
         <v>19</v>
       </c>
       <c r="C15" s="8">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D15" s="9">
-        <v>21.216666666666601</v>
+        <v>21.65</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" s="7">
-        <v>18</v>
+        <v>54</v>
       </c>
       <c r="C16" s="8">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D16" s="9">
-        <v>20.8333333333333</v>
+        <v>21.516666666666602</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B17" s="7">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="C17" s="8">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="D17" s="9">
-        <v>20.3333333333333</v>
+        <v>21.216666666666601</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="B18" s="7">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C18" s="8">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D18" s="9">
-        <v>19.9166666666666</v>
+        <v>20.8333333333333</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="B19" s="7">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="C19" s="8">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="D19" s="9">
-        <v>19.533333333333299</v>
+        <v>20.3333333333333</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>56</v>
+        <v>21</v>
+      </c>
+      <c r="B20" s="7">
+        <v>26</v>
       </c>
       <c r="C20" s="8">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="D20" s="9">
-        <v>18.600000000000001</v>
+        <v>19.9166666666666</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="B21" s="7">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="C21" s="8">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="D21" s="9">
-        <v>18.183333333333302</v>
+        <v>19.533333333333299</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B22" s="7">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="C22" s="8">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D22" s="9">
-        <v>17.5833333333333</v>
+        <v>18.600000000000001</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>49</v>
+        <v>19</v>
+      </c>
+      <c r="B23" s="7">
+        <v>8</v>
       </c>
       <c r="C23" s="8">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="D23" s="9">
-        <v>16.716666666666601</v>
+        <v>18.183333333333302</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="B24" s="7">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C24" s="8">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D24" s="9">
-        <v>15.25</v>
+        <v>17.5833333333333</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C25" s="8">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D25" s="9">
-        <v>15.05</v>
+        <v>16.716666666666601</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="B26" s="7">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C26" s="8">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D26" s="9">
-        <v>14.6</v>
+        <v>15.25</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C27" s="8">
         <v>18</v>
       </c>
       <c r="D27" s="9">
-        <v>13.65</v>
+        <v>15.05</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="B28" s="7">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C28" s="8">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D28" s="9">
-        <v>13.4166666666666</v>
+        <v>14.6</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B29" s="7">
-        <v>16</v>
+        <v>61</v>
       </c>
       <c r="C29" s="8">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D29" s="9">
-        <v>13.233333333333301</v>
+        <v>14.4333333333333</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C30" s="8">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D30" s="9">
-        <v>13.1833333333333</v>
+        <v>13.65</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B31" s="7">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C31" s="8">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D31" s="9">
-        <v>13.1166666666666</v>
+        <v>13.4166666666666</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>43</v>
+        <v>25</v>
+      </c>
+      <c r="B32" s="7">
+        <v>16</v>
       </c>
       <c r="C32" s="8">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D32" s="9">
-        <v>12.5833333333333</v>
+        <v>13.233333333333301</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B33" s="7">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="C33" s="8">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D33" s="9">
-        <v>12.283333333333299</v>
+        <v>13.1833333333333</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>45</v>
+        <v>30</v>
+      </c>
+      <c r="B34" s="7">
+        <v>14</v>
       </c>
       <c r="C34" s="8">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D34" s="9">
-        <v>11.8333333333333</v>
+        <v>13.1166666666666</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B35" s="7">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="C35" s="8">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D35" s="9">
-        <v>10.966666666666599</v>
+        <v>12.5833333333333</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="B36" s="7">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C36" s="8">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D36" s="9">
-        <v>9.85</v>
+        <v>12.283333333333299</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B37" s="7">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="C37" s="8">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D37" s="9">
-        <v>9.4166666666666607</v>
+        <v>11.8333333333333</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="B38" s="7">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C38" s="8">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D38" s="9">
-        <v>9.3333333333333304</v>
+        <v>10.966666666666599</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>48</v>
+        <v>32</v>
+      </c>
+      <c r="B39" s="7">
+        <v>11</v>
       </c>
       <c r="C39" s="8">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D39" s="9">
-        <v>8.75</v>
+        <v>9.85</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="B40" s="7">
         <v>11</v>
@@ -1136,37 +1151,37 @@
         <v>11</v>
       </c>
       <c r="D40" s="9">
-        <v>8.7333333333333307</v>
+        <v>9.4166666666666607</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="B41" s="7">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C41" s="8">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D41" s="9">
-        <v>8.43333333333333</v>
+        <v>9.3333333333333304</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C42" s="8">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D42" s="9">
-        <v>8.0500000000000007</v>
+        <v>8.75</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="B43" s="7">
         <v>11</v>
@@ -1175,160 +1190,243 @@
         <v>11</v>
       </c>
       <c r="D43" s="9">
-        <v>7.95</v>
+        <v>8.7333333333333307</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B44" s="7">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C44" s="8">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D44" s="9">
-        <v>7.7166666666666597</v>
+        <v>8.43333333333333</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C45" s="8">
         <v>10</v>
       </c>
       <c r="D45" s="9">
-        <v>7.4166666666666599</v>
+        <v>8.0500000000000007</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="B46" s="7">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C46" s="8">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D46" s="9">
-        <v>7.2166666666666597</v>
+        <v>7.95</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
-        <v>40</v>
+        <v>22</v>
+      </c>
+      <c r="B47" s="7">
+        <v>9</v>
       </c>
       <c r="C47" s="8">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D47" s="9">
-        <v>5.55</v>
+        <v>7.7166666666666597</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B48" s="7">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="C48" s="8">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D48" s="9">
-        <v>5.3833333333333302</v>
+        <v>7.4166666666666599</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="B49" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C49" s="8">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D49" s="9">
-        <v>5.36666666666666</v>
+        <v>7.2166666666666597</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B50" s="7">
-        <v>7</v>
+        <v>57</v>
       </c>
       <c r="C50" s="8">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D50" s="9">
-        <v>5.0166666666666604</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B51" s="7">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="C51" s="8">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D51" s="9">
-        <v>4.93333333333333</v>
+        <v>5.55</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="B52" s="7">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C52" s="8">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D52" s="9">
-        <v>3.85</v>
+        <v>5.3833333333333302</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B53" s="7">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C53" s="8">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D53" s="9">
-        <v>3.1</v>
+        <v>5.36666666666666</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B54" s="7">
+        <v>7</v>
+      </c>
+      <c r="C54" s="8">
+        <v>7</v>
+      </c>
+      <c r="D54" s="9">
+        <v>5.0166666666666604</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B55" s="7">
+        <v>5</v>
+      </c>
+      <c r="C55" s="8">
+        <v>5</v>
+      </c>
+      <c r="D55" s="9">
+        <v>4.93333333333333</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C56" s="8">
+        <v>5</v>
+      </c>
+      <c r="D56" s="9">
+        <v>4.8833333333333302</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C57" s="8">
+        <v>6</v>
+      </c>
+      <c r="D57" s="9">
+        <v>4.75</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B58" s="7">
+        <v>5</v>
+      </c>
+      <c r="C58" s="8">
+        <v>5</v>
+      </c>
+      <c r="D58" s="9">
+        <v>3.85</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C59" s="8">
+        <v>2</v>
+      </c>
+      <c r="D59" s="9">
+        <v>3.5333333333333301</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B60" s="7">
+        <v>2</v>
+      </c>
+      <c r="C60" s="8">
+        <v>3</v>
+      </c>
+      <c r="D60" s="9">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B54" s="7">
+      <c r="B61" s="7">
         <v>4</v>
       </c>
-      <c r="C54" s="8">
+      <c r="C61" s="8">
         <v>4</v>
       </c>
-      <c r="D54" s="9">
+      <c r="D61" s="9">
         <v>2.65</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D54">
-    <sortCondition descending="1" ref="D34:D54"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D61">
+    <sortCondition descending="1" ref="D37:D61"/>
   </sortState>
   <conditionalFormatting sqref="D1:D1048576">
     <cfRule type="colorScale" priority="2">

</xml_diff>

<commit_message>
game name path with colon fix setGameStatus add reset button setGameStatus add link near game time
</commit_message>
<xml_diff>
--- a/game time.xlsx
+++ b/game time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Program Files\HTML\Games\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7260B3AD-3F00-4D2B-98C0-7E62890C425B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96373E88-6E28-46A9-86F5-3B52F75BF0F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
   <si>
     <t>Игра</t>
   </si>
@@ -217,6 +217,9 @@
   </si>
   <si>
     <t>Outer Wilds</t>
+  </si>
+  <si>
+    <t>S.T.A.L.K.E.R.: Lost Alpha DC</t>
   </si>
 </sst>
 </file>
@@ -627,10 +630,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D61"/>
+  <dimension ref="A1:D62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="G66" sqref="G66"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -777,372 +780,369 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="7">
-        <v>11</v>
+        <v>64</v>
       </c>
       <c r="C12" s="8">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D12" s="9">
-        <v>23.933333333333302</v>
+        <v>26.6666666666666</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B13" s="7">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C13" s="8">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D13" s="9">
-        <v>22.5833333333333</v>
+        <v>23.933333333333302</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B14" s="7">
         <v>21</v>
       </c>
       <c r="C14" s="8">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D14" s="9">
-        <v>21.85</v>
+        <v>22.5833333333333</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="B15" s="7">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C15" s="8">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D15" s="9">
-        <v>21.65</v>
+        <v>21.85</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>54</v>
+        <v>31</v>
+      </c>
+      <c r="B16" s="7">
+        <v>19</v>
       </c>
       <c r="C16" s="8">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D16" s="9">
-        <v>21.516666666666602</v>
+        <v>21.65</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="7">
-        <v>19</v>
+        <v>54</v>
       </c>
       <c r="C17" s="8">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="D17" s="9">
-        <v>21.216666666666601</v>
+        <v>21.516666666666602</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="B18" s="7">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C18" s="8">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D18" s="9">
-        <v>20.8333333333333</v>
+        <v>21.216666666666601</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B19" s="7">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="C19" s="8">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="D19" s="9">
-        <v>20.3333333333333</v>
+        <v>20.8333333333333</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B20" s="7">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="C20" s="8">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="D20" s="9">
-        <v>19.9166666666666</v>
+        <v>20.3333333333333</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="B21" s="7">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C21" s="8">
         <v>26</v>
       </c>
       <c r="D21" s="9">
-        <v>19.533333333333299</v>
+        <v>19.9166666666666</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>56</v>
+        <v>39</v>
+      </c>
+      <c r="B22" s="7">
+        <v>23</v>
       </c>
       <c r="C22" s="8">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="D22" s="9">
-        <v>18.600000000000001</v>
+        <v>19.533333333333299</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B23" s="7">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="C23" s="8">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="D23" s="9">
-        <v>18.183333333333302</v>
+        <v>18.600000000000001</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B24" s="7">
+        <v>8</v>
+      </c>
+      <c r="C24" s="8">
         <v>10</v>
       </c>
-      <c r="C24" s="8">
-        <v>21</v>
-      </c>
       <c r="D24" s="9">
-        <v>17.5833333333333</v>
+        <v>18.183333333333302</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>49</v>
+        <v>11</v>
+      </c>
+      <c r="B25" s="7">
+        <v>10</v>
       </c>
       <c r="C25" s="8">
         <v>21</v>
       </c>
       <c r="D25" s="9">
-        <v>16.716666666666601</v>
+        <v>17.5833333333333</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B26" s="7">
-        <v>16</v>
+        <v>49</v>
       </c>
       <c r="C26" s="8">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D26" s="9">
-        <v>15.25</v>
+        <v>16.716666666666601</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>44</v>
+        <v>38</v>
+      </c>
+      <c r="B27" s="7">
+        <v>16</v>
       </c>
       <c r="C27" s="8">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D27" s="9">
-        <v>15.05</v>
+        <v>15.25</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B28" s="7">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="C28" s="8">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D28" s="9">
-        <v>14.6</v>
+        <v>15.05</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>61</v>
+        <v>15</v>
+      </c>
+      <c r="B29" s="7">
+        <v>13</v>
       </c>
       <c r="C29" s="8">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D29" s="9">
-        <v>14.4333333333333</v>
+        <v>14.6</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="C30" s="8">
         <v>18</v>
       </c>
       <c r="D30" s="9">
-        <v>13.65</v>
+        <v>14.4333333333333</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B31" s="7">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="C31" s="8">
         <v>18</v>
       </c>
       <c r="D31" s="9">
-        <v>13.4166666666666</v>
+        <v>13.65</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="B32" s="7">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C32" s="8">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D32" s="9">
-        <v>13.233333333333301</v>
+        <v>13.4166666666666</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>50</v>
+        <v>25</v>
+      </c>
+      <c r="B33" s="7">
+        <v>16</v>
       </c>
       <c r="C33" s="8">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D33" s="9">
-        <v>13.1833333333333</v>
+        <v>13.233333333333301</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B34" s="7">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="C34" s="8">
         <v>14</v>
       </c>
       <c r="D34" s="9">
-        <v>13.1166666666666</v>
+        <v>13.1833333333333</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>43</v>
+        <v>30</v>
+      </c>
+      <c r="B35" s="7">
+        <v>14</v>
       </c>
       <c r="C35" s="8">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D35" s="9">
-        <v>12.5833333333333</v>
+        <v>13.1166666666666</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B36" s="7">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="C36" s="8">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D36" s="9">
-        <v>12.283333333333299</v>
+        <v>12.5833333333333</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>45</v>
+        <v>5</v>
+      </c>
+      <c r="B37" s="7">
+        <v>8</v>
       </c>
       <c r="C37" s="8">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D37" s="9">
-        <v>11.8333333333333</v>
+        <v>12.283333333333299</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B38" s="7">
-        <v>13</v>
+        <v>45</v>
       </c>
       <c r="C38" s="8">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D38" s="9">
-        <v>10.966666666666599</v>
+        <v>11.8333333333333</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B39" s="7">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C39" s="8">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D39" s="9">
-        <v>9.85</v>
+        <v>10.966666666666599</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="B40" s="7">
         <v>11</v>
@@ -1151,282 +1151,296 @@
         <v>11</v>
       </c>
       <c r="D40" s="9">
-        <v>9.4166666666666607</v>
+        <v>9.85</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B41" s="7">
         <v>11</v>
       </c>
       <c r="C41" s="8">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D41" s="9">
-        <v>9.3333333333333304</v>
+        <v>9.4166666666666607</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>48</v>
+        <v>7</v>
+      </c>
+      <c r="B42" s="7">
+        <v>11</v>
       </c>
       <c r="C42" s="8">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D42" s="9">
-        <v>8.75</v>
+        <v>9.3333333333333304</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B43" s="7">
-        <v>11</v>
+        <v>48</v>
       </c>
       <c r="C43" s="8">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D43" s="9">
-        <v>8.7333333333333307</v>
+        <v>8.75</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B44" s="7">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C44" s="8">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D44" s="9">
-        <v>8.43333333333333</v>
+        <v>8.7333333333333307</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
-        <v>47</v>
+        <v>18</v>
+      </c>
+      <c r="B45" s="7">
+        <v>8</v>
       </c>
       <c r="C45" s="8">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D45" s="9">
-        <v>8.0500000000000007</v>
+        <v>8.43333333333333</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B46" s="7">
-        <v>11</v>
+        <v>47</v>
       </c>
       <c r="C46" s="8">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D46" s="9">
-        <v>7.95</v>
+        <v>8.0500000000000007</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="B47" s="7">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C47" s="8">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D47" s="9">
-        <v>7.7166666666666597</v>
+        <v>7.95</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
-        <v>41</v>
+        <v>22</v>
+      </c>
+      <c r="B48" s="7">
+        <v>9</v>
       </c>
       <c r="C48" s="8">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D48" s="9">
-        <v>7.4166666666666599</v>
+        <v>7.7166666666666597</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B49" s="7">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="C49" s="8">
         <v>10</v>
       </c>
       <c r="D49" s="9">
-        <v>7.2166666666666597</v>
+        <v>7.4166666666666599</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
-        <v>57</v>
+        <v>23</v>
+      </c>
+      <c r="B50" s="7">
+        <v>10</v>
       </c>
       <c r="C50" s="8">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D50" s="9">
-        <v>6.5</v>
+        <v>7.2166666666666597</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="C51" s="8">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D51" s="9">
-        <v>5.55</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B52" s="7">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="C52" s="8">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D52" s="9">
-        <v>5.3833333333333302</v>
+        <v>5.55</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="B53" s="7">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C53" s="8">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D53" s="9">
-        <v>5.36666666666666</v>
+        <v>5.3833333333333302</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="B54" s="7">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C54" s="8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D54" s="9">
-        <v>5.0166666666666604</v>
+        <v>5.36666666666666</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="B55" s="7">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C55" s="8">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D55" s="9">
-        <v>4.93333333333333</v>
+        <v>5.0166666666666604</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
-        <v>63</v>
+        <v>34</v>
+      </c>
+      <c r="B56" s="7">
+        <v>5</v>
       </c>
       <c r="C56" s="8">
         <v>5</v>
       </c>
       <c r="D56" s="9">
-        <v>4.8833333333333302</v>
+        <v>4.93333333333333</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C57" s="8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D57" s="9">
-        <v>4.75</v>
+        <v>4.8833333333333302</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B58" s="7">
-        <v>5</v>
+        <v>62</v>
       </c>
       <c r="C58" s="8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D58" s="9">
-        <v>3.85</v>
+        <v>4.75</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
-        <v>60</v>
+        <v>28</v>
+      </c>
+      <c r="B59" s="7">
+        <v>5</v>
       </c>
       <c r="C59" s="8">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D59" s="9">
-        <v>3.5333333333333301</v>
+        <v>3.85</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B60" s="7">
+        <v>60</v>
+      </c>
+      <c r="C60" s="8">
         <v>2</v>
       </c>
-      <c r="C60" s="8">
-        <v>3</v>
-      </c>
       <c r="D60" s="9">
-        <v>3.1</v>
+        <v>3.5333333333333301</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B61" s="7">
+        <v>2</v>
+      </c>
+      <c r="C61" s="8">
+        <v>3</v>
+      </c>
+      <c r="D61" s="9">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B61" s="7">
+      <c r="B62" s="7">
         <v>4</v>
       </c>
-      <c r="C61" s="8">
+      <c r="C62" s="8">
         <v>4</v>
       </c>
-      <c r="D61" s="9">
+      <c r="D62" s="9">
         <v>2.65</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D61">
-    <sortCondition descending="1" ref="D37:D61"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D62">
+    <sortCondition descending="1" ref="D43:D62"/>
   </sortState>
   <conditionalFormatting sqref="D1:D1048576">
     <cfRule type="colorScale" priority="2">

</xml_diff>

<commit_message>
setGameModal fix game time
</commit_message>
<xml_diff>
--- a/game time.xlsx
+++ b/game time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Program Files\HTML\Games\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96373E88-6E28-46A9-86F5-3B52F75BF0F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1159A559-5F2C-46D8-BA8F-D05C06D48DDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>Игра</t>
   </si>
@@ -220,6 +220,9 @@
   </si>
   <si>
     <t>S.T.A.L.K.E.R.: Lost Alpha DC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resident Evil 5 </t>
   </si>
 </sst>
 </file>
@@ -630,10 +633,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D62"/>
+  <dimension ref="A1:D63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1298,149 +1301,160 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="C52" s="8">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D52" s="9">
-        <v>5.55</v>
+        <v>6.3333333333333304</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B53" s="7">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="C53" s="8">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D53" s="9">
-        <v>5.3833333333333302</v>
+        <v>5.55</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="B54" s="7">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C54" s="8">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D54" s="9">
-        <v>5.36666666666666</v>
+        <v>5.3833333333333302</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="B55" s="7">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C55" s="8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D55" s="9">
-        <v>5.0166666666666604</v>
+        <v>5.36666666666666</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="B56" s="7">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C56" s="8">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D56" s="9">
-        <v>4.93333333333333</v>
+        <v>5.0166666666666604</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
-        <v>63</v>
+        <v>34</v>
+      </c>
+      <c r="B57" s="7">
+        <v>5</v>
       </c>
       <c r="C57" s="8">
         <v>5</v>
       </c>
       <c r="D57" s="9">
-        <v>4.8833333333333302</v>
+        <v>4.93333333333333</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C58" s="8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D58" s="9">
-        <v>4.75</v>
+        <v>4.8833333333333302</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B59" s="7">
-        <v>5</v>
+        <v>62</v>
       </c>
       <c r="C59" s="8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D59" s="9">
-        <v>3.85</v>
+        <v>4.75</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
-        <v>60</v>
+        <v>28</v>
+      </c>
+      <c r="B60" s="7">
+        <v>5</v>
       </c>
       <c r="C60" s="8">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D60" s="9">
-        <v>3.5333333333333301</v>
+        <v>3.85</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B61" s="7">
+        <v>60</v>
+      </c>
+      <c r="C61" s="8">
         <v>2</v>
       </c>
-      <c r="C61" s="8">
-        <v>3</v>
-      </c>
       <c r="D61" s="9">
-        <v>3.1</v>
+        <v>3.5333333333333301</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B62" s="7">
+        <v>2</v>
+      </c>
+      <c r="C62" s="8">
+        <v>3</v>
+      </c>
+      <c r="D62" s="9">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B62" s="7">
+      <c r="B63" s="7">
         <v>4</v>
       </c>
-      <c r="C62" s="8">
+      <c r="C63" s="8">
         <v>4</v>
       </c>
-      <c r="D62" s="9">
+      <c r="D63" s="9">
         <v>2.65</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D62">
-    <sortCondition descending="1" ref="D43:D62"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D63">
+    <sortCondition descending="1" ref="D40:D63"/>
   </sortState>
   <conditionalFormatting sqref="D1:D1048576">
     <cfRule type="colorScale" priority="2">

</xml_diff>

<commit_message>
Episode Choice Remake 3.0
</commit_message>
<xml_diff>
--- a/game time.xlsx
+++ b/game time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Program Files\HTML\Games\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1159A559-5F2C-46D8-BA8F-D05C06D48DDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1375AAA-FBF3-4343-9D9A-37A5C5CE576B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
   <si>
     <t>Игра</t>
   </si>
@@ -223,6 +223,21 @@
   </si>
   <si>
     <t xml:space="preserve">Resident Evil 5 </t>
+  </si>
+  <si>
+    <t>Atomic Heart</t>
+  </si>
+  <si>
+    <t>S.T.A.L.K.E.R.: Clear Sky</t>
+  </si>
+  <si>
+    <t>S.T.A.L.K.E.R.: Lost Alpha Enhanced Edition [ng++]</t>
+  </si>
+  <si>
+    <t>Dead Space</t>
+  </si>
+  <si>
+    <t>S.T.A.L.K.E.R.: Call of Pripyat Gunslinger</t>
   </si>
 </sst>
 </file>
@@ -633,10 +648,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D63"/>
+  <dimension ref="A1:D68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -822,383 +837,374 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="7">
-        <v>21</v>
+        <v>66</v>
       </c>
       <c r="C15" s="8">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D15" s="9">
-        <v>21.85</v>
+        <v>22.4166666666666</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="B16" s="7">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C16" s="8">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D16" s="9">
-        <v>21.65</v>
+        <v>21.85</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>54</v>
+        <v>31</v>
+      </c>
+      <c r="B17" s="7">
+        <v>19</v>
       </c>
       <c r="C17" s="8">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D17" s="9">
-        <v>21.516666666666602</v>
+        <v>21.65</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" s="7">
-        <v>19</v>
+        <v>54</v>
       </c>
       <c r="C18" s="8">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="D18" s="9">
-        <v>21.216666666666601</v>
+        <v>21.516666666666602</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="B19" s="7">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C19" s="8">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D19" s="9">
-        <v>20.8333333333333</v>
+        <v>21.216666666666601</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B20" s="7">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="C20" s="8">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="D20" s="9">
-        <v>20.3333333333333</v>
+        <v>20.8333333333333</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B21" s="7">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="C21" s="8">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="D21" s="9">
-        <v>19.9166666666666</v>
+        <v>20.3333333333333</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="B22" s="7">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C22" s="8">
         <v>26</v>
       </c>
       <c r="D22" s="9">
-        <v>19.533333333333299</v>
+        <v>19.9166666666666</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>56</v>
+        <v>39</v>
+      </c>
+      <c r="B23" s="7">
+        <v>23</v>
       </c>
       <c r="C23" s="8">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="D23" s="9">
-        <v>18.600000000000001</v>
+        <v>19.533333333333299</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B24" s="7">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="C24" s="8">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="D24" s="9">
-        <v>18.183333333333302</v>
+        <v>18.600000000000001</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B25" s="7">
+        <v>8</v>
+      </c>
+      <c r="C25" s="8">
         <v>10</v>
       </c>
-      <c r="C25" s="8">
-        <v>21</v>
-      </c>
       <c r="D25" s="9">
-        <v>17.5833333333333</v>
+        <v>18.183333333333302</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>49</v>
+        <v>11</v>
+      </c>
+      <c r="B26" s="7">
+        <v>10</v>
       </c>
       <c r="C26" s="8">
         <v>21</v>
       </c>
       <c r="D26" s="9">
-        <v>16.716666666666601</v>
+        <v>17.5833333333333</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B27" s="7">
-        <v>16</v>
+        <v>49</v>
       </c>
       <c r="C27" s="8">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D27" s="9">
-        <v>15.25</v>
+        <v>16.716666666666601</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>44</v>
+        <v>70</v>
       </c>
       <c r="C28" s="8">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D28" s="9">
-        <v>15.05</v>
+        <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="B29" s="7">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C29" s="8">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D29" s="9">
-        <v>14.6</v>
+        <v>15.25</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="C30" s="8">
         <v>18</v>
       </c>
       <c r="D30" s="9">
-        <v>14.4333333333333</v>
+        <v>15.05</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>52</v>
+        <v>15</v>
+      </c>
+      <c r="B31" s="7">
+        <v>13</v>
       </c>
       <c r="C31" s="8">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D31" s="9">
-        <v>13.65</v>
+        <v>14.6</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B32" s="7">
-        <v>7</v>
+        <v>61</v>
       </c>
       <c r="C32" s="8">
         <v>18</v>
       </c>
       <c r="D32" s="9">
-        <v>13.4166666666666</v>
+        <v>14.4333333333333</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B33" s="7">
-        <v>16</v>
+        <v>52</v>
       </c>
       <c r="C33" s="8">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D33" s="9">
-        <v>13.233333333333301</v>
+        <v>13.65</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>50</v>
+        <v>36</v>
+      </c>
+      <c r="B34" s="7">
+        <v>7</v>
       </c>
       <c r="C34" s="8">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D34" s="9">
-        <v>13.1833333333333</v>
+        <v>13.4166666666666</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B35" s="7">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C35" s="8">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D35" s="9">
-        <v>13.1166666666666</v>
+        <v>13.233333333333301</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="C36" s="8">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D36" s="9">
-        <v>12.5833333333333</v>
+        <v>13.1833333333333</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="B37" s="7">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C37" s="8">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D37" s="9">
-        <v>12.283333333333299</v>
+        <v>13.1166666666666</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C38" s="8">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D38" s="9">
-        <v>11.8333333333333</v>
+        <v>12.5833333333333</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B39" s="7">
-        <v>13</v>
+        <v>67</v>
       </c>
       <c r="C39" s="8">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D39" s="9">
-        <v>10.966666666666599</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="B40" s="7">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C40" s="8">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D40" s="9">
-        <v>9.85</v>
+        <v>12.283333333333299</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B41" s="7">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="C41" s="8">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D41" s="9">
-        <v>9.4166666666666607</v>
+        <v>11.8333333333333</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B42" s="7">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="C42" s="8">
         <v>13</v>
       </c>
       <c r="D42" s="9">
-        <v>9.3333333333333304</v>
+        <v>11.316666666666601</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
-        <v>48</v>
+        <v>29</v>
+      </c>
+      <c r="B43" s="7">
+        <v>13</v>
       </c>
       <c r="C43" s="8">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D43" s="9">
-        <v>8.75</v>
+        <v>10.966666666666599</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B44" s="7">
         <v>11</v>
@@ -1207,254 +1213,318 @@
         <v>11</v>
       </c>
       <c r="D44" s="9">
-        <v>8.7333333333333307</v>
+        <v>9.85</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B45" s="7">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C45" s="8">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D45" s="9">
-        <v>8.43333333333333</v>
+        <v>9.4166666666666607</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
-        <v>47</v>
+        <v>7</v>
+      </c>
+      <c r="B46" s="7">
+        <v>11</v>
       </c>
       <c r="C46" s="8">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D46" s="9">
-        <v>8.0500000000000007</v>
+        <v>9.3333333333333304</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B47" s="7">
-        <v>11</v>
+        <v>48</v>
       </c>
       <c r="C47" s="8">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D47" s="9">
-        <v>7.95</v>
+        <v>8.75</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B48" s="7">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C48" s="8">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D48" s="9">
-        <v>7.7166666666666597</v>
+        <v>8.7333333333333307</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
-        <v>41</v>
+        <v>18</v>
+      </c>
+      <c r="B49" s="7">
+        <v>8</v>
       </c>
       <c r="C49" s="8">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D49" s="9">
-        <v>7.4166666666666599</v>
+        <v>8.43333333333333</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B50" s="7">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="C50" s="8">
         <v>10</v>
       </c>
       <c r="D50" s="9">
-        <v>7.2166666666666597</v>
+        <v>8.0500000000000007</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
-        <v>57</v>
+        <v>6</v>
+      </c>
+      <c r="B51" s="7">
+        <v>11</v>
       </c>
       <c r="C51" s="8">
         <v>11</v>
       </c>
       <c r="D51" s="9">
-        <v>6.5</v>
+        <v>7.95</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
-        <v>65</v>
+        <v>22</v>
+      </c>
+      <c r="B52" s="7">
+        <v>9</v>
       </c>
       <c r="C52" s="8">
         <v>9</v>
       </c>
       <c r="D52" s="9">
-        <v>6.3333333333333304</v>
+        <v>7.7166666666666597</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="C53" s="8">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D53" s="9">
-        <v>5.55</v>
+        <v>7.4666666666666597</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B54" s="7">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="C54" s="8">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D54" s="9">
-        <v>5.3833333333333302</v>
+        <v>7.4166666666666599</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="B55" s="7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C55" s="8">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D55" s="9">
-        <v>5.36666666666666</v>
+        <v>7.2166666666666597</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B56" s="7">
-        <v>7</v>
+        <v>57</v>
       </c>
       <c r="C56" s="8">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D56" s="9">
-        <v>5.0166666666666604</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B57" s="7">
-        <v>5</v>
+        <v>65</v>
       </c>
       <c r="C57" s="8">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D57" s="9">
-        <v>4.93333333333333</v>
+        <v>6.3333333333333304</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="C58" s="8">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D58" s="9">
-        <v>4.8833333333333302</v>
+        <v>5.55</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
-        <v>62</v>
+        <v>17</v>
+      </c>
+      <c r="B59" s="7">
+        <v>8</v>
       </c>
       <c r="C59" s="8">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D59" s="9">
-        <v>4.75</v>
+        <v>5.3833333333333302</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="B60" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C60" s="8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D60" s="9">
-        <v>3.85</v>
+        <v>5.36666666666666</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
-        <v>60</v>
+        <v>10</v>
+      </c>
+      <c r="B61" s="7">
+        <v>7</v>
       </c>
       <c r="C61" s="8">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D61" s="9">
-        <v>3.5333333333333301</v>
+        <v>5.0166666666666604</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B62" s="7">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C62" s="8">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D62" s="9">
-        <v>3.1</v>
+        <v>4.93333333333333</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C63" s="8">
+        <v>5</v>
+      </c>
+      <c r="D63" s="9">
+        <v>4.8833333333333302</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C64" s="8">
+        <v>6</v>
+      </c>
+      <c r="D64" s="9">
+        <v>4.75</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B65" s="7">
+        <v>5</v>
+      </c>
+      <c r="C65" s="8">
+        <v>5</v>
+      </c>
+      <c r="D65" s="9">
+        <v>3.85</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C66" s="8">
+        <v>2</v>
+      </c>
+      <c r="D66" s="9">
+        <v>3.5333333333333301</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B67" s="7">
+        <v>2</v>
+      </c>
+      <c r="C67" s="8">
+        <v>3</v>
+      </c>
+      <c r="D67" s="9">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B63" s="7">
+      <c r="B68" s="7">
         <v>4</v>
       </c>
-      <c r="C63" s="8">
+      <c r="C68" s="8">
         <v>4</v>
       </c>
-      <c r="D63" s="9">
+      <c r="D68" s="9">
         <v>2.65</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D63">
-    <sortCondition descending="1" ref="D40:D63"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D68">
+    <sortCondition descending="1" ref="D43:D68"/>
   </sortState>
   <conditionalFormatting sqref="D1:D1048576">
     <cfRule type="colorScale" priority="2">

</xml_diff>

<commit_message>
fix: snowrunner live to video
</commit_message>
<xml_diff>
--- a/game time.xlsx
+++ b/game time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Program Files\HTML\Games\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1375AAA-FBF3-4343-9D9A-37A5C5CE576B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7647C9AB-2D2F-4E06-8082-C11ECE132C18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
   <si>
     <t>Игра</t>
   </si>
@@ -238,6 +238,9 @@
   </si>
   <si>
     <t>S.T.A.L.K.E.R.: Call of Pripyat Gunslinger</t>
+  </si>
+  <si>
+    <t>Dead Space 2</t>
   </si>
 </sst>
 </file>
@@ -648,10 +651,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D68"/>
+  <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="N63" sqref="N63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1360,171 +1363,182 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="C56" s="8">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D56" s="9">
-        <v>6.5</v>
+        <v>7.2</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C57" s="8">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D57" s="9">
-        <v>6.3333333333333304</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="C58" s="8">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D58" s="9">
-        <v>5.55</v>
+        <v>6.3333333333333304</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B59" s="7">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="C59" s="8">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D59" s="9">
-        <v>5.3833333333333302</v>
+        <v>5.55</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="B60" s="7">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C60" s="8">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D60" s="9">
-        <v>5.36666666666666</v>
+        <v>5.3833333333333302</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="B61" s="7">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C61" s="8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D61" s="9">
-        <v>5.0166666666666604</v>
+        <v>5.36666666666666</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="B62" s="7">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C62" s="8">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D62" s="9">
-        <v>4.93333333333333</v>
+        <v>5.0166666666666604</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
-        <v>63</v>
+        <v>34</v>
+      </c>
+      <c r="B63" s="7">
+        <v>5</v>
       </c>
       <c r="C63" s="8">
         <v>5</v>
       </c>
       <c r="D63" s="9">
-        <v>4.8833333333333302</v>
+        <v>4.93333333333333</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C64" s="8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D64" s="9">
-        <v>4.75</v>
+        <v>4.8833333333333302</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B65" s="7">
-        <v>5</v>
+        <v>62</v>
       </c>
       <c r="C65" s="8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D65" s="9">
-        <v>3.85</v>
+        <v>4.75</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="s">
-        <v>60</v>
+        <v>28</v>
+      </c>
+      <c r="B66" s="7">
+        <v>5</v>
       </c>
       <c r="C66" s="8">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D66" s="9">
-        <v>3.5333333333333301</v>
+        <v>3.85</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B67" s="7">
+        <v>60</v>
+      </c>
+      <c r="C67" s="8">
         <v>2</v>
       </c>
-      <c r="C67" s="8">
-        <v>3</v>
-      </c>
       <c r="D67" s="9">
-        <v>3.1</v>
+        <v>3.5333333333333301</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B68" s="7">
+        <v>2</v>
+      </c>
+      <c r="C68" s="8">
+        <v>3</v>
+      </c>
+      <c r="D68" s="9">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B68" s="7">
+      <c r="B69" s="7">
         <v>4</v>
       </c>
-      <c r="C68" s="8">
+      <c r="C69" s="8">
         <v>4</v>
       </c>
-      <c r="D68" s="9">
+      <c r="D69" s="9">
         <v>2.65</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D68">
-    <sortCondition descending="1" ref="D43:D68"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D69">
+    <sortCondition descending="1" ref="D46:D69"/>
   </sortState>
   <conditionalFormatting sqref="D1:D1048576">
     <cfRule type="colorScale" priority="2">

</xml_diff>